<commit_message>
start of software read me
</commit_message>
<xml_diff>
--- a/SonoRover One/software/example input/protocol template/template_protocol_input.xlsx
+++ b/SonoRover One/software/example input/protocol template/template_protocol_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/FUS_Initiative/Hydrophone measurements/!Protocol Template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radbouduniversiteit-my.sharepoint.com/personal/margely_cornelissen_ru_nl/Documents/Documenten/GitHub/repositories/Radboud-FUS-measurement-kit/SonoRover One/software/example input/protocol template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E28B081-C55F-8540-9054-580651125B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37280" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -262,8 +262,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="48880184" y="4081991"/>
-          <a:ext cx="6749072" cy="3705954"/>
+          <a:off x="48857959" y="4002616"/>
+          <a:ext cx="6739547" cy="3645629"/>
           <a:chOff x="1109936" y="2363691"/>
           <a:chExt cx="6875015" cy="3645629"/>
         </a:xfrm>
@@ -6676,9 +6676,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6716,7 +6716,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6822,7 +6822,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6964,7 +6964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6974,42 +6974,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="187.83203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="148.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="187.875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="148.125" style="4" customWidth="1"/>
     <col min="15" max="15" width="28" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.875" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="15.625" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -7170,22 +7170,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -7195,7 +7195,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -7205,7 +7205,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -7215,7 +7215,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -7225,7 +7225,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -7235,7 +7235,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -7245,7 +7245,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -7255,7 +7255,7 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -7265,7 +7265,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -7275,7 +7275,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" s="4"/>
     </row>
   </sheetData>
@@ -7301,26 +7301,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cb83fc2-d77f-46b4-9581-c00b781f61fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8754a512-6dec-483d-b5c6-7cffcc0d02c1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C12600718C676640B862E0AA4EBA4F75" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f5b5271ce1c64dd6d8fbb2a683be13c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9cb83fc2-d77f-46b4-9581-c00b781f61fd" xmlns:ns3="8754a512-6dec-483d-b5c6-7cffcc0d02c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3472f45d873750127c69500d0e5c45f1" ns2:_="" ns3:_="">
     <xsd:import namespace="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
@@ -7543,10 +7523,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cb83fc2-d77f-46b4-9581-c00b781f61fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8754a512-6dec-483d-b5c6-7cffcc0d02c1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C755C0B-1A1A-4CAB-AAB3-F18FC1BEB5C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3099BEFB-1261-4A7B-B1BD-10B30D1875E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
+    <ds:schemaRef ds:uri="8754a512-6dec-483d-b5c6-7cffcc0d02c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7563,20 +7574,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3099BEFB-1261-4A7B-B1BD-10B30D1875E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C755C0B-1A1A-4CAB-AAB3-F18FC1BEB5C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
-    <ds:schemaRef ds:uri="8754a512-6dec-483d-b5c6-7cffcc0d02c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add templates and modify readme
</commit_message>
<xml_diff>
--- a/SonoRover One/software/example input/protocol template/template_protocol_input.xlsx
+++ b/SonoRover One/software/example input/protocol template/template_protocol_input.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radbouduniversiteit-my.sharepoint.com/personal/margely_cornelissen_ru_nl/Documents/Documenten/GitHub/repositories/Radboud-FUS-measurement-kit/SonoRover One/software/example input/protocol template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E28B081-C55F-8540-9054-580651125B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_A032F6DB3BF3CF38219BB56A5F687AFCE06D3065" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{458121AD-B514-4998-B182-7B35C481BABD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,24 +65,6 @@
     <t>direction_columns</t>
   </si>
   <si>
-    <t>max. + x [mm] w.r.t. focal point</t>
-  </si>
-  <si>
-    <t>max. - x [mm] w.r.t. focal point</t>
-  </si>
-  <si>
-    <t>max. + y [mm] w.r.t. focal point</t>
-  </si>
-  <si>
-    <t>max. - y [mm] w.r.t. focal point</t>
-  </si>
-  <si>
-    <t>max. + z [mm] w.r.t. focal point</t>
-  </si>
-  <si>
-    <t>max. - z [mm] w.r.t. focal point</t>
-  </si>
-  <si>
     <t>-x</t>
   </si>
   <si>
@@ -98,16 +80,10 @@
     <t>Coordinates based on excel file or parameters on the right?</t>
   </si>
   <si>
-    <t>C:\Users\marge\OneDrive - Radboud Universiteit\Documenten\GitHub\repositories\characterization-scanning-software\NeuroFUS characterization\Characterization_input\250_26_203.xlsx</t>
-  </si>
-  <si>
     <t>Path and filename of Isppa to Global power conversion excel</t>
   </si>
   <si>
     <t>Path and filename of coordinate excel</t>
-  </si>
-  <si>
-    <t>Protocol</t>
   </si>
   <si>
     <t>Pulse Repetition Interval [ms]</t>
@@ -137,7 +113,31 @@
     <t>Amplitude [%] (fill in 'Corresponding value')</t>
   </si>
   <si>
-    <t>Z:\FUS_Initiative\Hydrophone measurements\!Coordinate Templates\1D\Axial_0_05_140mm\Axial_0_05_140mm.xls</t>
+    <t>max. + x [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>max. - x [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>max. + y [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>max. - y [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>max. + z [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>max. - z [mm] w.r.t. relative zero</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>C:\Temp\Characterization_input\250_26_203.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Temp\Radboud-FUS-measurement-kit\SonoRover One\software\example input\coordinate templates\1D\Axial_0_01_140mm\Axial_0_01_140mm.csv</t>
   </si>
 </sst>
 </file>
@@ -262,8 +262,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="48857959" y="4002616"/>
-          <a:ext cx="6739547" cy="3645629"/>
+          <a:off x="29925434" y="4634441"/>
+          <a:ext cx="6755422" cy="3705954"/>
           <a:chOff x="1109936" y="2363691"/>
           <a:chExt cx="6875015" cy="3645629"/>
         </a:xfrm>
@@ -6676,9 +6676,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6716,7 +6716,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6822,7 +6822,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6964,7 +6964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6974,31 +6974,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="187.875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="33.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="148.125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="52.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.75" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.75" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.875" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="27.5" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.125" style="3" bestFit="1" customWidth="1"/>
@@ -7011,64 +7011,64 @@
   <sheetData>
     <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>6</v>
@@ -7089,7 +7089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -7116,19 +7116,19 @@
         <v>200</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3">
-        <v>2500</v>
+        <v>40</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L2" s="3">
         <v>44</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>33</v>
@@ -7152,13 +7152,13 @@
         <v>0</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="X2" s="3">
         <v>5</v>
@@ -7280,18 +7280,18 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"'+x,'-x,'+y,'-y,'+z,'-z"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{35EACE7F-184C-46F6-B30C-1D4825B6758C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Coordinate excel file, Parameters on the right"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{013D177A-98B8-423F-905E-6C2C411F9647}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Amplitude [%] (fill in 'Corresponding value'),Global power [mW] (fill in 'Corresponding value'),Isppa [W/cm2] (fill in 'Corresponding value' and 'Excel path and filename of Isppa to Global power conversion table'),"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Square,Linear,Tukey,Logarithmic,Exponential,Gaussian"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+      <formula1>"Square,Linear,Tukey,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7301,6 +7301,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cb83fc2-d77f-46b4-9581-c00b781f61fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8754a512-6dec-483d-b5c6-7cffcc0d02c1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C12600718C676640B862E0AA4EBA4F75" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f5b5271ce1c64dd6d8fbb2a683be13c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9cb83fc2-d77f-46b4-9581-c00b781f61fd" xmlns:ns3="8754a512-6dec-483d-b5c6-7cffcc0d02c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3472f45d873750127c69500d0e5c45f1" ns2:_="" ns3:_="">
     <xsd:import namespace="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
@@ -7523,27 +7543,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cb83fc2-d77f-46b4-9581-c00b781f61fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8754a512-6dec-483d-b5c6-7cffcc0d02c1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C755C0B-1A1A-4CAB-AAB3-F18FC1BEB5C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{363ED61F-1B79-49C7-A484-F44EFFCDAAF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
+    <ds:schemaRef ds:uri="8754a512-6dec-483d-b5c6-7cffcc0d02c1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3099BEFB-1261-4A7B-B1BD-10B30D1875E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7560,23 +7579,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{363ED61F-1B79-49C7-A484-F44EFFCDAAF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9cb83fc2-d77f-46b4-9581-c00b781f61fd"/>
-    <ds:schemaRef ds:uri="8754a512-6dec-483d-b5c6-7cffcc0d02c1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C755C0B-1A1A-4CAB-AAB3-F18FC1BEB5C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>